<commit_message>
change parser output template as well as minor file reader fix
</commit_message>
<xml_diff>
--- a/testExcel.xlsx
+++ b/testExcel.xlsx
@@ -375,78 +375,228 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>invoice_number</v>
+        <v>SEQ_NO(M)</v>
       </c>
       <c r="B1" t="str">
-        <v>order_number</v>
+        <v>HOUSE_BL_NO(M)</v>
       </c>
       <c r="C1" t="str">
-        <v>invoice_date</v>
+        <v>SHIPMENT_DATE(YYYYMMDD)(M)</v>
       </c>
       <c r="D1" t="str">
-        <v>due_date</v>
+        <v>ARRIVAL_DATE(YYYYMMDD)(M)</v>
       </c>
       <c r="E1" t="str">
-        <v>tax</v>
+        <v>SHIPMENT_COUNTRY_CODE(M)</v>
       </c>
       <c r="F1" t="str">
-        <v>total_due</v>
+        <v>SHIPMENT_METHOD_CODE(M)</v>
       </c>
       <c r="G1" t="str">
-        <v>bank</v>
+        <v>ARRIVAL_PORT_CODE(M)</v>
       </c>
       <c r="H1" t="str">
-        <v>account</v>
+        <v>PRICE_TERMS_CODE(M)</v>
       </c>
       <c r="I1" t="str">
-        <v>bsb</v>
+        <v>SHIPMENT_CURRENCY_CODE(M)</v>
       </c>
       <c r="J1" t="str">
-        <v>remarks</v>
+        <v>FINAL_DESTINATION_CODE(M)</v>
+      </c>
+      <c r="K1" t="str">
+        <v>LINE_NUM(M)</v>
+      </c>
+      <c r="L1" t="str">
+        <v>ITEM_NO(M)</v>
+      </c>
+      <c r="M1" t="str">
+        <v>QUANTITY_SHIPPED(M)</v>
+      </c>
+      <c r="N1" t="str">
+        <v>UNIT_PRICE(M)</v>
+      </c>
+      <c r="O1" t="str">
+        <v>VAT_AMOUNT</v>
+      </c>
+      <c r="P1" t="str">
+        <v>IMPORT_DECLARATION_NO</v>
+      </c>
+      <c r="Q1" t="str">
+        <v>IMPORT_DECLARATION_DATE(YYYYMMDD)</v>
+      </c>
+      <c r="R1" t="str">
+        <v>CC_AMOUNT</v>
+      </c>
+      <c r="S1" t="str">
+        <v>DUTY_AMOUNT</v>
+      </c>
+      <c r="T1" t="str">
+        <v>SHIPMENT_PORT_CODE</v>
+      </c>
+      <c r="U1" t="str">
+        <v>PACKING_QTY</v>
+      </c>
+      <c r="V1" t="str">
+        <v>PACKING_UNIT_CODE</v>
+      </c>
+      <c r="W1" t="str">
+        <v>CARGO_TYPE_CODE</v>
+      </c>
+      <c r="X1" t="str">
+        <v>TOTAL_CBM</v>
+      </c>
+      <c r="Y1" t="str">
+        <v>GROSS_WEIGHT</v>
+      </c>
+      <c r="Z1" t="str">
+        <v>CHARGEABLE_WEIGHT</v>
+      </c>
+      <c r="AA1" t="str">
+        <v>GROSS_WEIGHT_UOM_CODE</v>
+      </c>
+      <c r="AB1" t="str">
+        <v>VESSEL_FLIGHT_NAME</v>
+      </c>
+      <c r="AC1" t="str">
+        <v>VENDOR_SITE_CODE</v>
+      </c>
+      <c r="AD1" t="str">
+        <v>COURIER_FLAG</v>
+      </c>
+      <c r="AE1" t="str">
+        <v>ITEM_SPEC</v>
+      </c>
+      <c r="AF1" t="str">
+        <v>HS_NO</v>
+      </c>
+      <c r="AG1" t="str">
+        <v>UNIT_OF_MEASURE</v>
+      </c>
+      <c r="AH1" t="str">
+        <v>CC_COUNTRY_CODE</v>
+      </c>
+      <c r="AI1" t="str">
+        <v>ORGANIZATION_CODE</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>INV-3337</v>
+        <v/>
       </c>
       <c r="B2" t="str">
-        <v>12345</v>
+        <v>2395544244</v>
       </c>
       <c r="C2" t="str">
-        <v>January 25, 2016</v>
+        <v/>
       </c>
       <c r="D2" t="str">
-        <v>January 31, 2016</v>
+        <v/>
       </c>
       <c r="E2" t="str">
-        <v>$8.50</v>
+        <v>KR</v>
       </c>
       <c r="F2" t="str">
-        <v>$93.50</v>
+        <v/>
       </c>
       <c r="G2" t="str">
-        <v>ANZ Bank</v>
+        <v>DEMUC</v>
       </c>
       <c r="H2" t="str">
-        <v>ACC # 1234 1234</v>
+        <v>DAP</v>
       </c>
       <c r="I2" t="str">
-        <v>BSB # 4321 432</v>
+        <v/>
       </c>
       <c r="J2" t="str">
-        <v>Payment is due within 30 days from date of invoice. Late payment is subject to fees of 5% per month.</v>
+        <v>DEMUC</v>
+      </c>
+      <c r="K2" t="str">
+        <v/>
+      </c>
+      <c r="L2" t="str">
+        <v>LGE CID G01 10.25 APX2T FST</v>
+      </c>
+      <c r="M2" t="str">
+        <v/>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <v>996,68</v>
+      </c>
+      <c r="P2" t="str">
+        <v>ATC00400931750820195604</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>20190819</v>
+      </c>
+      <c r="R2" t="str">
+        <v>5.117,76</v>
+      </c>
+      <c r="S2" t="str">
+        <v>127,94</v>
+      </c>
+      <c r="T2" t="str">
+        <v/>
+      </c>
+      <c r="U2" t="str">
+        <v/>
+      </c>
+      <c r="V2" t="str">
+        <v/>
+      </c>
+      <c r="W2" t="str">
+        <v/>
+      </c>
+      <c r="X2" t="str">
+        <v/>
+      </c>
+      <c r="Y2" t="str">
+        <v/>
+      </c>
+      <c r="Z2" t="str">
+        <v/>
+      </c>
+      <c r="AA2" t="str">
+        <v/>
+      </c>
+      <c r="AB2" t="str">
+        <v/>
+      </c>
+      <c r="AC2" t="str">
+        <v/>
+      </c>
+      <c r="AD2" t="str">
+        <v/>
+      </c>
+      <c r="AE2" t="str">
+        <v/>
+      </c>
+      <c r="AF2" t="str">
+        <v>85299092990</v>
+      </c>
+      <c r="AG2" t="str">
+        <v/>
+      </c>
+      <c r="AH2" t="str">
+        <v/>
+      </c>
+      <c r="AI2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AI2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add reading multiple files and work on row creation in excel
</commit_message>
<xml_diff>
--- a/testExcel.xlsx
+++ b/testExcel.xlsx
@@ -492,7 +492,7 @@
         <v/>
       </c>
       <c r="B2" t="str">
-        <v>2395544244</v>
+        <v>2395540825</v>
       </c>
       <c r="C2" t="str">
         <v/>
@@ -522,7 +522,7 @@
         <v/>
       </c>
       <c r="L2" t="str">
-        <v>LGE CID G01 10.25 APX2T FST</v>
+        <v>: HEAD-UP-DISPLAY</v>
       </c>
       <c r="M2" t="str">
         <v/>
@@ -531,19 +531,19 @@
         <v/>
       </c>
       <c r="O2" t="str">
-        <v>996,68</v>
+        <v>587,91</v>
       </c>
       <c r="P2" t="str">
-        <v>ATC00400931750820195604</v>
+        <v>ATC00401281230820195604</v>
       </c>
       <c r="Q2" t="str">
-        <v>20190819</v>
+        <v>20190826</v>
       </c>
       <c r="R2" t="str">
-        <v>5.117,76</v>
+        <v>3012.93</v>
       </c>
       <c r="S2" t="str">
-        <v>127,94</v>
+        <v>81,35</v>
       </c>
       <c r="T2" t="str">
         <v/>
@@ -582,7 +582,7 @@
         <v/>
       </c>
       <c r="AF2" t="str">
-        <v>85299092990</v>
+        <v>85122000900</v>
       </c>
       <c r="AG2" t="str">
         <v/>

</xml_diff>